<commit_message>
1º só q amaerlo
é igual ao primeiro só que amarelo
</commit_message>
<xml_diff>
--- a/teste git.xlsx
+++ b/teste git.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>só isso no priemeiro momento</t>
-  </si>
-  <si>
-    <t>na segunda tem isso</t>
   </si>
 </sst>
 </file>
@@ -35,12 +32,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +58,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,22 +365,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1º só que vermelho
igual ao primeiro só que vermelho
</commit_message>
<xml_diff>
--- a/teste git.xlsx
+++ b/teste git.xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>só isso no priemeiro momento</t>
-  </si>
-  <si>
-    <t>na segunda tem isso</t>
   </si>
 </sst>
 </file>
@@ -35,12 +32,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +58,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -361,22 +365,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tentativa de escrever no pach vermelho
tentativa de escrever no pach vermelho
</commit_message>
<xml_diff>
--- a/teste git.xlsx
+++ b/teste git.xlsx
@@ -19,7 +19,7 @@
     <t>só isso no priemeiro momento</t>
   </si>
   <si>
-    <t>na segunda tem isso</t>
+    <t>vai</t>
   </si>
 </sst>
 </file>
@@ -35,12 +35,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -55,8 +61,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,7 +377,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>